<commit_message>
new files added and some updated
</commit_message>
<xml_diff>
--- a/bin/com/testdata/HalfEbayTestData.xlsx
+++ b/bin/com/testdata/HalfEbayTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{71353B8B-2C9E-4553-B27A-42A85E538C8E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9FF64366-5179-4468-9284-3D466A3413E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28860" windowHeight="16500" xr2:uid="{EB9354D6-7697-4B41-867F-C7F9EFFB93C7}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28980" windowHeight="16500" xr2:uid="{EB9354D6-7697-4B41-867F-C7F9EFFB93C7}"/>
   </bookViews>
   <sheets>
     <sheet name="RegTestData" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>sunny</t>
   </si>
   <si>
-    <t>california</t>
-  </si>
-  <si>
     <t>tom@gmail.com</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Rm@gmail.com</t>
+  </si>
+  <si>
+    <t>California</t>
   </si>
 </sst>
 </file>
@@ -160,10 +160,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,14 +483,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D129BE-EE79-4E60-A3AC-5B7538764640}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="8" max="8" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -505,7 +508,7 @@
       <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -529,97 +532,97 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G2">
         <v>94085</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G3">
         <v>94086</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G4">
         <v>94087</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G5">
         <v>94088</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>